<commit_message>
Fine-tune gen AI outputs
</commit_message>
<xml_diff>
--- a/Prompt Engineering/prompt library.xlsx
+++ b/Prompt Engineering/prompt library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mansi.P\OneDrive - AFour Technologies Pvt. Ltd\Desktop\AI\Notes\Notes\Prompt Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BC2F74F-5E27-491B-97AB-BE420483D132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E14C8B-84D5-49F4-811C-47606860DDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t xml:space="preserve">INSTRUCTIONS: As you complete the course, add your favorite and most effective prompts to your own personal prompt library. </t>
   </si>
@@ -146,6 +145,18 @@
   </si>
   <si>
     <t xml:space="preserve">Create meeting minutes for this meeting. Create sections based on key points extracted from the minutes. Attribute each key point to a speaker, and then assign action items to the speaker who is most appropriate to complete them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> My data set is a spreadsheet [add type of data here] that uses the following columns: [Mention column names here] Title, Published, Genre, First published, and Approximate sales in millions. Give me options for a chart that shows the correlation between genre and sales. Explain how genre and sales are correlated according to the information.</t>
+  </si>
+  <si>
+    <t>I am interested in showing the relationship between genre and sales. And the task. Suggest modifications to make this chart work better with my specific data using Google Sheets.</t>
+  </si>
+  <si>
+    <t>I'm a product designer at a headphones brand. I am putting together a presentation for my team about what new features should be included in our next product line. The presentation includes findings from our market research on features that our 18 to 34 year old customers want their headphones to have. These features include new colours, the ability to control playback with head movements, and noise-cancelling capabilities. consider the relationship between our demographics` disposable income and their most important considerations when buying headphones. How should I structure my presentation? List each slide's topic with its key points and visuals.</t>
+  </si>
+  <si>
+    <t>generate close-up images of a pair of sleek silver headphone on a desk in a college dorm room. They should have musical notes floating around the headphones to show that they're playing music.</t>
   </si>
 </sst>
 </file>
@@ -510,8 +521,8 @@
   </sheetPr>
   <dimension ref="A1:AA991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -835,11 +846,15 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
     </row>
-    <row r="9" spans="1:27" ht="30" customHeight="1">
-      <c r="A9" s="6"/>
+    <row r="9" spans="1:27" ht="80" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B9" s="6"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -864,11 +879,15 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
     </row>
-    <row r="10" spans="1:27" ht="30" customHeight="1">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:27" ht="137.5">
+      <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>

</xml_diff>